<commit_message>
Updated the testcase document.
</commit_message>
<xml_diff>
--- a/testplan/ticket_service_testcases.xlsx
+++ b/testplan/ticket_service_testcases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560"/>
+    <workbookView xWindow="-35420" yWindow="360" windowWidth="27960" windowHeight="18640"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Test cases</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Date test</t>
   </si>
   <si>
     <t>Find the number of the available seats</t>
@@ -174,10 +171,16 @@
     <t>Verify the return code is 403 after Reserve and commit the held seats for the different customers when the holds exp</t>
   </si>
   <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
     <t>Verify the number of the available seats are equal to xx in Level x after hold the seats for the customer</t>
+  </si>
+  <si>
+    <t>Actually Result</t>
+  </si>
+  <si>
+    <t>Test execution date</t>
+  </si>
+  <si>
+    <t>Bug#</t>
   </si>
 </sst>
 </file>
@@ -596,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -608,11 +611,13 @@
     <col min="2" max="2" width="79.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -629,513 +634,562 @@
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18">
+      <c r="A2" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="15">
+      <c r="G2" s="9"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="2"/>
       <c r="B3" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="15">
+      <c r="G3" s="4"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="15">
+      <c r="G4" s="4"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="2"/>
       <c r="B5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="15">
+      <c r="G5" s="4"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="2"/>
       <c r="B6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="15">
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15">
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" s="2"/>
       <c r="B9" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="30">
+      <c r="G9" s="4"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="30">
+      <c r="G10" s="4"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="15">
+      <c r="G11" s="4"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="15">
+      <c r="G12" s="4"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15">
+      <c r="G13" s="4"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="2"/>
       <c r="B14" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15">
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="2"/>
       <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="18">
+      <c r="G15" s="4"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="18">
       <c r="A16" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15">
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="15">
+      <c r="G17" s="4"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="15">
+      <c r="G18" s="4"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="60">
+      <c r="G19" s="4"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" ht="60">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="30">
+      <c r="G20" s="4"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" ht="30">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="15">
+      <c r="G21" s="4"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="15">
+      <c r="G22" s="4"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="60">
+      <c r="G23" s="4"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="60">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="30">
+      <c r="G24" s="4"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="30">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="15">
+      <c r="G25" s="4"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="30">
+      <c r="G26" s="4"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="30">
       <c r="A27" s="2"/>
       <c r="B27" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="30">
+      <c r="G27" s="4"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="30">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="30">
+      <c r="G28" s="4"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="30">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="15">
+      <c r="G29" s="4"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="15">
+      <c r="G30" s="4"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="15">
+      <c r="G31" s="4"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" ht="15">
+      <c r="G32" s="4"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="15">
+      <c r="G33" s="4"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" ht="18">
+      <c r="G34" s="4"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" ht="18">
       <c r="A35" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="30">
+      <c r="G35" s="9"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" ht="30">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" ht="30">
+      <c r="G36" s="4"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" ht="30">
       <c r="A37" s="2"/>
       <c r="B37" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="30">
+      <c r="G37" s="4"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" ht="30">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" ht="45">
+      <c r="G38" s="4"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" ht="45">
       <c r="A39" s="2"/>
       <c r="B39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" ht="30">
+      <c r="G39" s="4"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" ht="30">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" ht="30">
+      <c r="G40" s="4"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" ht="30">
       <c r="A41" s="2"/>
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" ht="30">
+      <c r="G41" s="4"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="30">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" ht="30">
+      <c r="G42" s="4"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" ht="30">
       <c r="A43" s="2"/>
       <c r="B43" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" ht="30">
+      <c r="G43" s="4"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" ht="30">
       <c r="A44" s="2"/>
       <c r="B44" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" ht="45">
+      <c r="G44" s="4"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" ht="45">
       <c r="A45" s="2"/>
       <c r="B45" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" ht="30">
+      <c r="G45" s="4"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" ht="30">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" ht="30">
+      <c r="G46" s="4"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8" ht="30">
       <c r="A47" s="2"/>
       <c r="B47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>